<commit_message>
new files and project
</commit_message>
<xml_diff>
--- a/week2/corr_matrix.xlsx
+++ b/week2/corr_matrix.xlsx
@@ -955,40 +955,40 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.1021467709075159</v>
+        <v>0.1</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>0.9453089324427374</v>
+        <v>0.95</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>0.297298834334204</v>
+        <v>0.3</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>0.04603587445988568</v>
+        <v>0.05</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>-0.01104068187161769</v>
+        <v>-0.01</v>
       </c>
       <c r="H2" s="8" t="n">
-        <v>0.393135377530929</v>
+        <v>0.39</v>
       </c>
       <c r="I2" s="9" t="n">
-        <v>0.1036482628791938</v>
+        <v>0.1</v>
       </c>
       <c r="J2" s="10" t="n">
-        <v>-0.176329818995305</v>
+        <v>-0.18</v>
       </c>
       <c r="K2" s="11" t="n">
-        <v>-0.2004123368439069</v>
+        <v>-0.2</v>
       </c>
       <c r="L2" s="10" t="n">
-        <v>-0.07392631232580818</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="M2" s="12" t="n">
-        <v>0.3444412485549885</v>
+        <v>0.34</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>0.1022405628705482</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3">
@@ -998,43 +998,43 @@
         </is>
       </c>
       <c r="B3" s="13" t="n">
-        <v>0.1021467709075159</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.1285187268715931</v>
+        <v>0.13</v>
       </c>
       <c r="E3" s="14" t="n">
-        <v>-0.07404981090670515</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="F3" s="9" t="n">
-        <v>0.1319594400471236</v>
+        <v>0.13</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>0.05832370940096267</v>
+        <v>0.06</v>
       </c>
       <c r="H3" s="12" t="n">
-        <v>0.3720647458980499</v>
+        <v>0.37</v>
       </c>
       <c r="I3" s="16" t="n">
-        <v>-0.0122091683458227</v>
+        <v>-0.01</v>
       </c>
       <c r="J3" s="17" t="n">
-        <v>0.07875414180374476</v>
+        <v>0.08</v>
       </c>
       <c r="K3" s="10" t="n">
-        <v>-0.2469071299907494</v>
+        <v>-0.25</v>
       </c>
       <c r="L3" s="18" t="n">
-        <v>-0.05368355289671318</v>
+        <v>-0.05</v>
       </c>
       <c r="M3" s="19" t="n">
-        <v>-0.08313109601691224</v>
+        <v>-0.08</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0.9978585860741387</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1044,43 +1044,43 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.9453089324427374</v>
+        <v>0.95</v>
       </c>
       <c r="C4" s="20" t="n">
-        <v>0.1285187268715931</v>
+        <v>0.13</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="21" t="n">
-        <v>0.287981054055412</v>
+        <v>0.29</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0.04623952257356188</v>
+        <v>0.05</v>
       </c>
       <c r="G4" s="22" t="n">
-        <v>0.001215039258107744</v>
+        <v>0</v>
       </c>
       <c r="H4" s="23" t="n">
-        <v>0.137494058292969</v>
+        <v>0.14</v>
       </c>
       <c r="I4" s="23" t="n">
-        <v>0.08873800149996208</v>
+        <v>0.09</v>
       </c>
       <c r="J4" s="24" t="n">
-        <v>-0.1408714696870539</v>
+        <v>-0.14</v>
       </c>
       <c r="K4" s="24" t="n">
-        <v>-0.2110019269867617</v>
+        <v>-0.21</v>
       </c>
       <c r="L4" s="10" t="n">
-        <v>-0.07316814497049197</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="M4" s="25" t="n">
-        <v>0.3321697575118642</v>
+        <v>0.33</v>
       </c>
       <c r="N4" s="26" t="n">
-        <v>0.1283334616436006</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="5">
@@ -1090,43 +1090,43 @@
         </is>
       </c>
       <c r="B5" s="27" t="n">
-        <v>0.297298834334204</v>
+        <v>0.3</v>
       </c>
       <c r="C5" s="28" t="n">
-        <v>-0.07404981090670515</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D5" s="29" t="n">
-        <v>0.287981054055412</v>
+        <v>0.29</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="n">
-        <v>-0.1267396223152305</v>
+        <v>-0.13</v>
       </c>
       <c r="G5" s="30" t="n">
-        <v>0.04288707095725015</v>
+        <v>0.04</v>
       </c>
       <c r="H5" s="31" t="n">
-        <v>0.05278313320678397</v>
+        <v>0.05</v>
       </c>
       <c r="I5" s="32" t="n">
-        <v>0.09909932699272071</v>
+        <v>0.1</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>-0.1371766794940462</v>
+        <v>-0.14</v>
       </c>
       <c r="K5" s="33" t="n">
-        <v>-0.03106072146176578</v>
+        <v>-0.03</v>
       </c>
       <c r="L5" s="34" t="n">
-        <v>0.006112339236423578</v>
+        <v>0.01</v>
       </c>
       <c r="M5" s="35" t="n">
-        <v>0.9641466077247648</v>
+        <v>0.96</v>
       </c>
       <c r="N5" s="28" t="n">
-        <v>-0.0737202560795321</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -1136,43 +1136,43 @@
         </is>
       </c>
       <c r="B6" s="36" t="n">
-        <v>0.04603587445988568</v>
+        <v>0.05</v>
       </c>
       <c r="C6" s="20" t="n">
-        <v>0.1319594400471236</v>
+        <v>0.13</v>
       </c>
       <c r="D6" s="37" t="n">
-        <v>0.04623952257356188</v>
+        <v>0.05</v>
       </c>
       <c r="E6" s="38" t="n">
-        <v>-0.1267396223152305</v>
+        <v>-0.13</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="24" t="n">
-        <v>-0.0136642330691138</v>
+        <v>-0.01</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v>0.06507627179428081</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I6" s="16" t="n">
-        <v>-0.0136945035062699</v>
+        <v>-0.01</v>
       </c>
       <c r="J6" s="39" t="n">
-        <v>-0.02813406487205172</v>
+        <v>-0.03</v>
       </c>
       <c r="K6" s="28" t="n">
-        <v>-0.07317198649379532</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="L6" s="24" t="n">
-        <v>-0.04329727449083477</v>
+        <v>-0.04</v>
       </c>
       <c r="M6" s="40" t="n">
-        <v>-0.1311392409110284</v>
+        <v>-0.13</v>
       </c>
       <c r="N6" s="20" t="n">
-        <v>0.1318215110261589</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="7">
@@ -1182,43 +1182,43 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>-0.01104068187161769</v>
+        <v>-0.01</v>
       </c>
       <c r="C7" s="41" t="n">
-        <v>0.05832370940096267</v>
+        <v>0.06</v>
       </c>
       <c r="D7" s="33" t="n">
-        <v>0.001215039258107744</v>
+        <v>0</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>0.04288707095725015</v>
+        <v>0.04</v>
       </c>
       <c r="F7" s="42" t="n">
-        <v>-0.0136642330691138</v>
+        <v>-0.01</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="43" t="n">
-        <v>-0.0121446746351008</v>
+        <v>-0.01</v>
       </c>
       <c r="I7" s="44" t="n">
-        <v>0.03100631566569882</v>
+        <v>0.03</v>
       </c>
       <c r="J7" s="45" t="n">
-        <v>-0.045327763422312</v>
+        <v>-0.05</v>
       </c>
       <c r="K7" s="46" t="n">
-        <v>-0.01763454297559341</v>
+        <v>-0.02</v>
       </c>
       <c r="L7" s="47" t="n">
-        <v>-0.00798993518586417</v>
+        <v>-0.01</v>
       </c>
       <c r="M7" s="48" t="n">
-        <v>0.04930656854045498</v>
+        <v>0.05</v>
       </c>
       <c r="N7" s="41" t="n">
-        <v>0.05708483842855755</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
@@ -1228,43 +1228,43 @@
         </is>
       </c>
       <c r="B8" s="49" t="n">
-        <v>0.393135377530929</v>
+        <v>0.39</v>
       </c>
       <c r="C8" s="50" t="n">
-        <v>0.3720647458980499</v>
+        <v>0.37</v>
       </c>
       <c r="D8" s="51" t="n">
-        <v>0.137494058292969</v>
+        <v>0.14</v>
       </c>
       <c r="E8" s="52" t="n">
-        <v>0.05278313320678397</v>
+        <v>0.05</v>
       </c>
       <c r="F8" s="33" t="n">
-        <v>0.06507627179428081</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>-0.0121446746351008</v>
+        <v>-0.01</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="I8" s="53" t="n">
-        <v>0.06738236204432484</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J8" s="14" t="n">
-        <v>-0.1091022715865082</v>
+        <v>-0.11</v>
       </c>
       <c r="K8" s="54" t="n">
-        <v>-0.09701652299419762</v>
+        <v>-0.1</v>
       </c>
       <c r="L8" s="55" t="n">
-        <v>-0.05079277033164126</v>
+        <v>-0.05</v>
       </c>
       <c r="M8" s="56" t="n">
-        <v>0.06297683070964306</v>
+        <v>0.06</v>
       </c>
       <c r="N8" s="49" t="n">
-        <v>0.3718044608098892</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="9">
@@ -1274,43 +1274,43 @@
         </is>
       </c>
       <c r="B9" s="13" t="n">
-        <v>0.1036482628791938</v>
+        <v>0.1</v>
       </c>
       <c r="C9" s="57" t="n">
-        <v>-0.0122091683458227</v>
+        <v>-0.01</v>
       </c>
       <c r="D9" s="58" t="n">
-        <v>0.08873800149996208</v>
+        <v>0.09</v>
       </c>
       <c r="E9" s="59" t="n">
-        <v>0.09909932699272071</v>
+        <v>0.1</v>
       </c>
       <c r="F9" s="42" t="n">
-        <v>-0.0136945035062699</v>
+        <v>-0.01</v>
       </c>
       <c r="G9" s="60" t="n">
-        <v>0.03100631566569882</v>
+        <v>0.03</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v>0.06738236204432484</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="J9" s="61" t="n">
-        <v>-0.1698912051175176</v>
+        <v>-0.17</v>
       </c>
       <c r="K9" s="37" t="n">
-        <v>0.01698734166940071</v>
+        <v>0.02</v>
       </c>
       <c r="L9" s="11" t="n">
-        <v>-0.03591009402995616</v>
+        <v>-0.04</v>
       </c>
       <c r="M9" s="9" t="n">
-        <v>0.1104257452179065</v>
+        <v>0.11</v>
       </c>
       <c r="N9" s="46" t="n">
-        <v>-0.0128425615782073</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="10">
@@ -1320,43 +1320,43 @@
         </is>
       </c>
       <c r="B10" s="55" t="n">
-        <v>-0.176329818995305</v>
+        <v>-0.18</v>
       </c>
       <c r="C10" s="62" t="n">
-        <v>0.07875414180374476</v>
+        <v>0.08</v>
       </c>
       <c r="D10" s="14" t="n">
-        <v>-0.1408714696870539</v>
+        <v>-0.14</v>
       </c>
       <c r="E10" s="10" t="n">
-        <v>-0.1371766794940462</v>
+        <v>-0.14</v>
       </c>
       <c r="F10" s="63" t="n">
-        <v>-0.02813406487205172</v>
+        <v>-0.03</v>
       </c>
       <c r="G10" s="10" t="n">
-        <v>-0.045327763422312</v>
+        <v>-0.05</v>
       </c>
       <c r="H10" s="10" t="n">
-        <v>-0.1091022715865082</v>
+        <v>-0.11</v>
       </c>
       <c r="I10" s="10" t="n">
-        <v>-0.1698912051175176</v>
+        <v>-0.17</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="K10" s="59" t="n">
-        <v>0.0126182140084551</v>
+        <v>0.01</v>
       </c>
       <c r="L10" s="64" t="n">
-        <v>0.0398155387592887</v>
+        <v>0.04</v>
       </c>
       <c r="M10" s="10" t="n">
-        <v>-0.1616126998212074</v>
+        <v>-0.16</v>
       </c>
       <c r="N10" s="62" t="n">
-        <v>0.07855289098027267</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="11">
@@ -1366,43 +1366,43 @@
         </is>
       </c>
       <c r="B11" s="10" t="n">
-        <v>-0.2004123368439069</v>
+        <v>-0.2</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>-0.2469071299907494</v>
+        <v>-0.25</v>
       </c>
       <c r="D11" s="10" t="n">
-        <v>-0.2110019269867617</v>
+        <v>-0.21</v>
       </c>
       <c r="E11" s="63" t="n">
-        <v>-0.03106072146176578</v>
+        <v>-0.03</v>
       </c>
       <c r="F11" s="65" t="n">
-        <v>-0.07317198649379532</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="G11" s="40" t="n">
-        <v>-0.01763454297559341</v>
+        <v>-0.02</v>
       </c>
       <c r="H11" s="38" t="n">
-        <v>-0.09701652299419762</v>
+        <v>-0.1</v>
       </c>
       <c r="I11" s="6" t="n">
-        <v>0.01698734166940071</v>
+        <v>0.02</v>
       </c>
       <c r="J11" s="66" t="n">
-        <v>0.0126182140084551</v>
+        <v>0.01</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="30" t="n">
-        <v>0.01822163545245604</v>
+        <v>0.02</v>
       </c>
       <c r="M11" s="45" t="n">
-        <v>-0.03351895205199327</v>
+        <v>-0.03</v>
       </c>
       <c r="N11" s="10" t="n">
-        <v>-0.2444684699671112</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="12">
@@ -1412,43 +1412,43 @@
         </is>
       </c>
       <c r="B12" s="42" t="n">
-        <v>-0.07392631232580818</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="C12" s="67" t="n">
-        <v>-0.05368355289671318</v>
+        <v>-0.05</v>
       </c>
       <c r="D12" s="68" t="n">
-        <v>-0.07316814497049197</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="E12" s="39" t="n">
-        <v>0.006112339236423578</v>
+        <v>0.01</v>
       </c>
       <c r="F12" s="34" t="n">
-        <v>-0.04329727449083477</v>
+        <v>-0.04</v>
       </c>
       <c r="G12" s="11" t="n">
-        <v>-0.00798993518586417</v>
+        <v>-0.01</v>
       </c>
       <c r="H12" s="65" t="n">
-        <v>-0.05079277033164126</v>
+        <v>-0.05</v>
       </c>
       <c r="I12" s="68" t="n">
-        <v>-0.03591009402995616</v>
+        <v>-0.04</v>
       </c>
       <c r="J12" s="46" t="n">
-        <v>0.0398155387592887</v>
+        <v>0.04</v>
       </c>
       <c r="K12" s="37" t="n">
-        <v>0.01822163545245604</v>
+        <v>0.02</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="M12" s="31" t="n">
-        <v>0.006697191266571591</v>
+        <v>0.01</v>
       </c>
       <c r="N12" s="67" t="n">
-        <v>-0.05316245044678064</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="13">
@@ -1458,43 +1458,43 @@
         </is>
       </c>
       <c r="B13" s="69" t="n">
-        <v>0.3444412485549885</v>
+        <v>0.34</v>
       </c>
       <c r="C13" s="70" t="n">
-        <v>-0.08313109601691224</v>
+        <v>-0.08</v>
       </c>
       <c r="D13" s="71" t="n">
-        <v>0.3321697575118642</v>
+        <v>0.33</v>
       </c>
       <c r="E13" s="72" t="n">
-        <v>0.9641466077247648</v>
+        <v>0.96</v>
       </c>
       <c r="F13" s="10" t="n">
-        <v>-0.1311392409110284</v>
+        <v>-0.13</v>
       </c>
       <c r="G13" s="63" t="n">
-        <v>0.04930656854045498</v>
+        <v>0.05</v>
       </c>
       <c r="H13" s="67" t="n">
-        <v>0.06297683070964306</v>
+        <v>0.06</v>
       </c>
       <c r="I13" s="73" t="n">
-        <v>0.1104257452179065</v>
+        <v>0.11</v>
       </c>
       <c r="J13" s="74" t="n">
-        <v>-0.1616126998212074</v>
+        <v>-0.16</v>
       </c>
       <c r="K13" s="44" t="n">
-        <v>-0.03351895205199327</v>
+        <v>-0.03</v>
       </c>
       <c r="L13" s="34" t="n">
-        <v>0.006697191266571591</v>
+        <v>0.01</v>
       </c>
       <c r="M13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="N13" s="70" t="n">
-        <v>-0.08280156884856611</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="14">
@@ -1504,40 +1504,40 @@
         </is>
       </c>
       <c r="B14" s="13" t="n">
-        <v>0.1022405628705482</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.9978585860741387</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>0.1283334616436006</v>
+        <v>0.13</v>
       </c>
       <c r="E14" s="14" t="n">
-        <v>-0.0737202560795321</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="F14" s="9" t="n">
-        <v>0.1318215110261589</v>
+        <v>0.13</v>
       </c>
       <c r="G14" s="15" t="n">
-        <v>0.05708483842855755</v>
+        <v>0.06</v>
       </c>
       <c r="H14" s="12" t="n">
-        <v>0.3718044608098892</v>
+        <v>0.37</v>
       </c>
       <c r="I14" s="16" t="n">
-        <v>-0.0128425615782073</v>
+        <v>-0.01</v>
       </c>
       <c r="J14" s="17" t="n">
-        <v>0.07855289098027267</v>
+        <v>0.08</v>
       </c>
       <c r="K14" s="10" t="n">
-        <v>-0.2444684699671112</v>
+        <v>-0.24</v>
       </c>
       <c r="L14" s="18" t="n">
-        <v>-0.05316245044678064</v>
+        <v>-0.05</v>
       </c>
       <c r="M14" s="19" t="n">
-        <v>-0.08280156884856611</v>
+        <v>-0.08</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>1</v>

</xml_diff>